<commit_message>
Updated Names to ue, ss, ae
</commit_message>
<xml_diff>
--- a/ImmmoWelt_Price_Guide/data/flats_to_rent_wue_preprocessed_combined.xlsx
+++ b/ImmmoWelt_Price_Guide/data/flats_to_rent_wue_preprocessed_combined.xlsx
@@ -79,7 +79,7 @@
     <t>dusche</t>
   </si>
   <si>
-    <t>einbauk\u00fcche</t>
+    <t>einbaukueche</t>
   </si>
   <si>
     <t>elektro</t>
@@ -115,7 +115,7 @@
     <t>frei</t>
   </si>
   <si>
-    <t>fu\u00dfbodenheizung</t>
+    <t>fussbodenheizung</t>
   </si>
   <si>
     <t>gaestewc</t>
@@ -163,7 +163,7 @@
     <t>klimatisiert</t>
   </si>
   <si>
-    <t>kontrollierte_be-_und_entl\u00fcftungsanlage</t>
+    <t>kontrollierte_be-_und_entlueftungsanlage</t>
   </si>
   <si>
     <t>kunststoff</t>
@@ -205,7 +205,7 @@
     <t>ofenheizung</t>
   </si>
   <si>
-    <t>offene_k\u00fcche</t>
+    <t>offene_kueche</t>
   </si>
   <si>
     <t>pantry</t>
@@ -241,7 +241,7 @@
     <t>stellplatz</t>
   </si>
   <si>
-    <t>teilweise_m\u00f6bliert</t>
+    <t>teilweise_moebliert</t>
   </si>
   <si>
     <t>teppich</t>

</xml_diff>